<commit_message>
Add files for search using budget
</commit_message>
<xml_diff>
--- a/Excelfiles/testdata.xlsx
+++ b/Excelfiles/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dissanayake\Desktop\PythonSelenium\BDD\PythonPageObjectModel\Excelfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B00C5FA-5833-4223-80A1-0DF75DD2A433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC8B81F-4079-4A92-A8F7-E95C8CB127C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B63C629F-968E-4D73-97E0-3300776CE5D3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{B63C629F-968E-4D73-97E0-3300776CE5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="logintest" sheetId="1" r:id="rId1"/>
     <sheet name="carbrandtest" sheetId="2" r:id="rId2"/>
+    <sheet name="filtercars" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>phone_no</t>
   </si>
@@ -119,6 +120,9 @@
   </si>
   <si>
     <t>BMW Cars</t>
+  </si>
+  <si>
+    <t>BMW</t>
   </si>
 </sst>
 </file>
@@ -578,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F39C1FAA-C42E-4285-8EF3-42D3E56E6D9F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -630,4 +634,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1FDA3B-04BF-4B70-BDFC-AB2E4DAFF84F}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>